<commit_message>
BAMM and niche conservatism updates
</commit_message>
<xml_diff>
--- a/niche_conserve_ancestral_recon/niche_conserve.xlsx
+++ b/niche_conserve_ancestral_recon/niche_conserve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfolk/Documents/GitHub/astragalus_niche_biogeo/niche_conserve_ancestral_recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B396DCDD-9FE8-8E4E-B180-BF6E01534D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD49F1D9-F9FD-2340-8DA0-B817258970B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{AD79B426-0962-174D-86C8-F9901F246AF6}"/>
+    <workbookView xWindow="3220" yWindow="2420" windowWidth="28040" windowHeight="17040" xr2:uid="{AD79B426-0962-174D-86C8-F9901F246AF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Variable</t>
   </si>
@@ -56,6 +56,30 @@
   </si>
   <si>
     <t>aridity</t>
+  </si>
+  <si>
+    <t>BIO4</t>
+  </si>
+  <si>
+    <t>BIO7</t>
+  </si>
+  <si>
+    <t>BIO12</t>
+  </si>
+  <si>
+    <t>BIO15</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>nitrogen</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>P (hochberg-corrected)</t>
   </si>
 </sst>
 </file>
@@ -408,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97EF405-668B-C645-9D22-08A7F8037B4E}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +450,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -437,8 +464,11 @@
       <c r="C2" s="1">
         <v>1.13812E-48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>1.026E-47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -448,8 +478,11 @@
       <c r="C3" s="1">
         <v>4.2750000000000001E-122</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>4.28E-121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -459,16 +492,120 @@
       <c r="C4" s="1">
         <v>1.8553E-134</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D4" s="1">
+        <v>2.0459999999999999E-133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.75571699999999997</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.7908199999999999E-42</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.2320000000000001E-41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.68789599999999995</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5.7569500000000002E-30</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.8800000000000002E-29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.585947</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.00525E-13</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.01E-13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.71018000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.6742200000000001E-26</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0100000000000002E-26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.85695200000000005</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.4637700000000001E-35</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.022E-34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.54563399999999995</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.9351200000000001E-29</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.7599999999999995E-29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.31294300000000003</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.5869299999999998E-24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7.1799999999999995E-24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B20">
+      <c r="B12">
         <v>0.63764799999999999</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C12" s="1">
         <v>8.4531000000000004E-31</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0700000000000003E-30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>